<commit_message>
fix bug client add album
</commit_message>
<xml_diff>
--- a/UML.xlsx
+++ b/UML.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daonhuanh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\C0821I1_LeVuDuy\Module Advanced Programming with Java\case-study-module-advanced-programming-with-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6298C6-76D8-9540-B9FE-7714709F0B11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB30A304-433F-493A-B0A6-0F2B6004C99F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="500" windowWidth="32080" windowHeight="20500" activeTab="3" xr2:uid="{EC98B4A8-BC12-40FB-ABF8-F7C1FC854E56}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EC98B4A8-BC12-40FB-ABF8-F7C1FC854E56}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>Interface</t>
   </si>
@@ -228,13 +228,25 @@
     <t>Làm xong 1 chức năng thì thử luôn</t>
   </si>
   <si>
-    <t>Accout</t>
-  </si>
-  <si>
-    <t>Accout manage</t>
-  </si>
-  <si>
     <t>GeneralService</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>8/11 - 9/11</t>
+  </si>
+  <si>
+    <t>Client service</t>
+  </si>
+  <si>
+    <t>+ Login / Register</t>
+  </si>
+  <si>
+    <t>+ Singleton</t>
+  </si>
+  <si>
+    <t>+ IO DataClient</t>
   </si>
 </sst>
 </file>
@@ -672,20 +684,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE81EE35-8E2F-4635-8A4A-5AF4B0F04DAA}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScale="255" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="255" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="35.5" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="3.5" customWidth="1"/>
-    <col min="7" max="7" width="3.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -697,7 +709,7 @@
       </c>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>10</v>
       </c>
@@ -709,7 +721,7 @@
       </c>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>46</v>
       </c>
@@ -721,7 +733,7 @@
       </c>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="12" t="s">
         <v>59</v>
@@ -731,7 +743,7 @@
       </c>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="12" t="s">
         <v>49</v>
@@ -741,11 +753,11 @@
       </c>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -753,7 +765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -764,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -775,7 +787,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>55</v>
       </c>
@@ -783,7 +795,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>54</v>
       </c>
@@ -791,7 +803,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>53</v>
       </c>
@@ -799,17 +811,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>58</v>
       </c>
@@ -828,31 +840,31 @@
       <selection activeCell="B3" sqref="B3:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.1640625" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="41.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" customWidth="1"/>
     <col min="5" max="5" width="2.6640625" customWidth="1"/>
     <col min="6" max="6" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -864,7 +876,7 @@
       </c>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>44</v>
       </c>
@@ -873,7 +885,7 @@
       </c>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>61</v>
       </c>
@@ -882,7 +894,7 @@
       </c>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>62</v>
       </c>
@@ -891,7 +903,7 @@
       </c>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
@@ -900,7 +912,7 @@
       </c>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
@@ -909,7 +921,7 @@
       </c>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>60</v>
       </c>
@@ -918,84 +930,84 @@
       </c>
       <c r="F10" s="15"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F11" s="16"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F12" s="16"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
         <v>63</v>
       </c>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F20" s="15"/>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="15"/>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D23" s="2" t="s">
         <v>60</v>
       </c>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F24" s="16"/>
     </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F26" s="16"/>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
       <c r="F27" s="16"/>
     </row>
   </sheetData>
@@ -1012,14 +1024,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="67.83203125" customWidth="1"/>
-    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="1" max="1" width="67.77734375" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -1027,7 +1039,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -1035,7 +1047,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -1043,7 +1055,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>39</v>
       </c>
@@ -1051,7 +1063,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -1059,7 +1071,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
@@ -1067,7 +1079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
@@ -1075,67 +1087,67 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
@@ -1148,28 +1160,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20CC3F53-0D7F-4B4D-9E1D-216A3B4A145D}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="180" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" customWidth="1"/>
     <col min="4" max="4" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1177,7 +1189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1188,141 +1200,157 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>26</v>
       </c>
     </row>

</xml_diff>